<commit_message>
Change xml element name of "Function".
</commit_message>
<xml_diff>
--- a/doc/sample/test_sample_input/google_test_sample_data_002.xlsx
+++ b/doc/sample/test_sample_input/google_test_sample_data_002.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="882"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="882" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="テスト一覧" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="242">
   <si>
     <t>○対象関数情報</t>
     <rPh sb="1" eb="7">
@@ -1031,6 +1031,10 @@
   </si>
   <si>
     <t>E:\development\AutoTestPrep\doc\sample\test_sample_input\sample_src_006.cpp</t>
+  </si>
+  <si>
+    <t>○テスト/デシジョンテーブル</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -1522,7 +1526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1676,7 +1680,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1821,7 +1827,7 @@
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.15">
       <c r="L9" s="10" t="s">
-        <v>32</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update sample codes. Update sample codes the application generates.
</commit_message>
<xml_diff>
--- a/doc/sample/test_sample_input/google_test_sample_data_002.xlsx
+++ b/doc/sample/test_sample_input/google_test_sample_data_002.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="882" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="882"/>
   </bookViews>
   <sheets>
     <sheet name="テスト一覧" sheetId="2" r:id="rId1"/>
@@ -1526,7 +1526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G9"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1680,9 +1680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>